<commit_message>
updates excel with ecoinvent 3.9 codes
</commit_message>
<xml_diff>
--- a/Course-material/test_db_excel_w_ecoinvent.xlsx
+++ b/Course-material/test_db_excel_w_ecoinvent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/massimo/Documents/AAU/Teaching/Courses/2020/2020_PhD_Advanced_LCA/Lectures/Module1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/massimo/Documents/AAU/Teaching/Courses/2023/Module2/Course-material/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEECF53-1074-7F43-B6F6-567169671197}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A328A070-4630-2F45-81D1-C37A9AF8011E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test0" sheetId="1" r:id="rId1"/>
@@ -129,17 +129,17 @@
     <t>kilowatt hour</t>
   </si>
   <si>
-    <t>2956c82487a849d85f353af64d37396e</t>
-  </si>
-  <si>
-    <t>ecoinvent 3.6 conseq</t>
+    <t>ecoinvent 3.9 conseq</t>
+  </si>
+  <si>
+    <t>cea1e434115aa84cbfd7dc3086b61e80</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -455,10 +455,10 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18.5" bestFit="1" customWidth="1"/>
@@ -476,7 +476,7 @@
     <col min="15" max="15" width="64.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -523,7 +523,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -555,7 +555,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -599,7 +599,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
@@ -646,7 +646,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
@@ -690,7 +690,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -722,7 +722,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
@@ -739,10 +739,10 @@
         <v>8</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="H7">
         <v>100</v>
@@ -757,7 +757,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -789,7 +789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
@@ -821,7 +821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -853,7 +853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>31</v>
       </c>
@@ -870,7 +870,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>31</v>
       </c>

</xml_diff>